<commit_message>
actualizamos el excel de condiciones
</commit_message>
<xml_diff>
--- a/planeacion.xlsx
+++ b/planeacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos_BD\DF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD230B7-3BAF-4CEE-B4D3-75571AC27FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E0C1AF-4133-4C9A-8638-2F38716A1537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{573208B1-CBA7-4B07-A7EC-C49677EEAD7B}"/>
   </bookViews>
@@ -425,55 +425,58 @@
   <dimension ref="B2:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B11" sqref="B2:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="1"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+    </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>